<commit_message>
teszt jegyzokonyvek befejezese soapui tesztek modositasa
</commit_message>
<xml_diff>
--- a/other/doc/Lightweight_Integration_TEST_v1_0.xlsx
+++ b/other/doc/Lightweight_Integration_TEST_v1_0.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="229">
   <si>
     <t>#</t>
   </si>
@@ -650,12 +650,191 @@
   <si>
     <t>Set the validation type to no</t>
   </si>
+  <si>
+    <t>Optional message validation, full soap message validation, message standard validation.
+CTX - newOSB</t>
+  </si>
+  <si>
+    <t>LWI HelloService TestSuit</t>
+  </si>
+  <si>
+    <t>Run the SayHello Test</t>
+  </si>
+  <si>
+    <t>Remove the ctx attributes from the first tag</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;lwit:helloLwi </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> RequestId="123456" CorrelationId="co555111" UserId="soapui-tester"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Run the SayHelloHeader Test</t>
+  </si>
+  <si>
+    <t>Remove the ctx header attributes from the request</t>
+  </si>
+  <si>
+    <t>Optional message validation, full soap message validation, message standard validation.
+CTX - XML attribute</t>
+  </si>
+  <si>
+    <t>Open test suits</t>
+  </si>
+  <si>
+    <t>cnr.getMsisdn
+  threads: 8
+  strategy: simple
+  testdelay: 500
+  random: 0.5
+  limit: 60 seconds</t>
+  </si>
+  <si>
+    <t>Set the request limit to 10</t>
+  </si>
+  <si>
+    <t>&lt;param name="maxRequest" value="10"/&gt;
+&lt;param name="queueSize" value="1"/&gt;</t>
+  </si>
+  <si>
+    <t>ESTORE getDocument TestSuite</t>
+  </si>
+  <si>
+    <t>load test runs without error</t>
+  </si>
+  <si>
+    <t>Raise the test therad number tu 12</t>
+  </si>
+  <si>
+    <t>threads=12</t>
+  </si>
+  <si>
+    <t>Continue the test</t>
+  </si>
+  <si>
+    <t>Couple of error happens</t>
+  </si>
+  <si>
+    <t>&lt;request-limit name="FULL_REQUEST_LIMIT" max-concurrent-requests="50" queue-size="1"/&gt;</t>
+  </si>
+  <si>
+    <t>sets</t>
+  </si>
+  <si>
+    <t>Set the request limit to 10 for getMsisdn</t>
+  </si>
+  <si>
+    <t>Set the request limit to 10 for estore qpdl</t>
+  </si>
+  <si>
+    <t>cnr.getMsisdn
+  threads: 10
+  strategy: simple
+  testdelay: 500
+  random: 0.5
+  limit: 60 seconds
+estore.qpdl
+  threads: 10
+  strategy: simple
+  testdelay: 500
+  random: 0.5
+  limit: 60 seconds</t>
+  </si>
+  <si>
+    <t>ESTORE qpdl TestSuite
+CNR getMsisdn TestSuit</t>
+  </si>
+  <si>
+    <t>Set load test params</t>
+  </si>
+  <si>
+    <t>Start the getMsisdn test</t>
+  </si>
+  <si>
+    <t>Runs without error</t>
+  </si>
+  <si>
+    <t>Stop the qpdl test</t>
+  </si>
+  <si>
+    <t>Stop the getMsisdn test</t>
+  </si>
+  <si>
+    <t>Stops</t>
+  </si>
+  <si>
+    <t>Start the qpdl test</t>
+  </si>
+  <si>
+    <t>Start both</t>
+  </si>
+  <si>
+    <t>Couple of both tests fail</t>
+  </si>
+  <si>
+    <t>Set FULL_REQUEST_LIMIT=12</t>
+  </si>
+  <si>
+    <t>Open all test suits</t>
+  </si>
+  <si>
+    <t>ESTORE qpdl TestSuite
+CNR getMsisdn TestSuit
+ESTORE getDocument TestSuite
+LWI HelloService TestSuit</t>
+  </si>
+  <si>
+    <t>for all the same
+  threads:20
+  strategy: simple
+  testdelay: 500
+  random: 0.5
+  limit: 60 seconds</t>
+  </si>
+  <si>
+    <t>Set the request limit to 20 for all plus 10 for queue size</t>
+  </si>
+  <si>
+    <t>&lt;param name="maxRequest" value="20"/&gt;
+&lt;param name="queueSize" value="10"/&gt;</t>
+  </si>
+  <si>
+    <t>Set FULL_REQUEST_LIMIT=100</t>
+  </si>
+  <si>
+    <t>&lt;request-limit name="FULL_REQUEST_LIMIT" max-concurrent-requests="100" queue-size="50"/&gt;</t>
+  </si>
+  <si>
+    <t>start the load</t>
+  </si>
+  <si>
+    <t>RUNS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -815,6 +994,13 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="238"/>
     </font>
   </fonts>
@@ -1249,7 +1435,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1331,6 +1517,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1387,18 +1594,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -1743,8 +1938,8 @@
   </sheetPr>
   <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="12.75"/>
@@ -1762,49 +1957,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" customFormat="1" ht="21" customHeight="1">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:8" customFormat="1" ht="21" customHeight="1">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="43" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="44"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="33"/>
+      <c r="G2" s="40"/>
     </row>
     <row r="3" spans="1:8" customFormat="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="47"/>
+      <c r="C3" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="44"/>
+      <c r="D3" s="51"/>
       <c r="E3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="34">
+      <c r="F3" s="41">
         <v>42624</v>
       </c>
-      <c r="G3" s="35"/>
+      <c r="G3" s="42"/>
     </row>
     <row r="4" spans="1:8" customFormat="1" ht="12" customHeight="1">
       <c r="A4" s="5"/>
@@ -1816,15 +2011,15 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="9" t="s">
@@ -1872,7 +2067,7 @@
         <v>102</v>
       </c>
       <c r="G7" s="29"/>
-      <c r="H7" s="20"/>
+      <c r="H7" s="37"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="38.25">
       <c r="A8" s="14" t="s">
@@ -1894,7 +2089,7 @@
         <v>41</v>
       </c>
       <c r="G8" s="29"/>
-      <c r="H8" s="20"/>
+      <c r="H8" s="37"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="76.5">
       <c r="A9" s="14" t="s">
@@ -1916,7 +2111,7 @@
         <v>42</v>
       </c>
       <c r="G9" s="29"/>
-      <c r="H9" s="20"/>
+      <c r="H9" s="37"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="76.5">
       <c r="A10" s="14" t="s">
@@ -1938,7 +2133,7 @@
         <v>42</v>
       </c>
       <c r="G10" s="29"/>
-      <c r="H10" s="20"/>
+      <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="76.5">
       <c r="A11" s="14" t="s">
@@ -1960,7 +2155,7 @@
         <v>42</v>
       </c>
       <c r="G11" s="29"/>
-      <c r="H11" s="20"/>
+      <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A12" s="14" t="s">
@@ -1982,7 +2177,7 @@
         <v>58</v>
       </c>
       <c r="G12" s="29"/>
-      <c r="H12" s="53"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A13" s="14" t="s">
@@ -2004,7 +2199,7 @@
         <v>58</v>
       </c>
       <c r="G13" s="29"/>
-      <c r="H13" s="52"/>
+      <c r="H13" s="36"/>
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" ht="102">
       <c r="A14" s="14" t="s">
@@ -2026,7 +2221,7 @@
         <v>70</v>
       </c>
       <c r="G14" s="29"/>
-      <c r="H14" s="52"/>
+      <c r="H14" s="36"/>
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" ht="102">
       <c r="A15" s="14" t="s">
@@ -2048,7 +2243,7 @@
         <v>70</v>
       </c>
       <c r="G15" s="29"/>
-      <c r="H15" s="52"/>
+      <c r="H15" s="36"/>
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A16" s="14" t="s">
@@ -2070,7 +2265,7 @@
         <v>81</v>
       </c>
       <c r="G16" s="29"/>
-      <c r="H16" s="20"/>
+      <c r="H16" s="36"/>
     </row>
     <row r="17" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A17" s="14" t="s">
@@ -2092,7 +2287,7 @@
         <v>81</v>
       </c>
       <c r="G17" s="29"/>
-      <c r="H17" s="20"/>
+      <c r="H17" s="37"/>
     </row>
     <row r="18" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A18" s="14" t="s">
@@ -2114,7 +2309,7 @@
         <v>81</v>
       </c>
       <c r="G18" s="29"/>
-      <c r="H18" s="20"/>
+      <c r="H18" s="37"/>
     </row>
     <row r="19" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A19" s="14" t="s">
@@ -2136,7 +2331,7 @@
         <v>81</v>
       </c>
       <c r="G19" s="29"/>
-      <c r="H19" s="20"/>
+      <c r="H19" s="37"/>
     </row>
     <row r="20" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A20" s="14" t="s">
@@ -2158,7 +2353,7 @@
         <v>81</v>
       </c>
       <c r="G20" s="11"/>
-      <c r="H20" s="20"/>
+      <c r="H20" s="36"/>
     </row>
     <row r="21" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A21" s="14" t="s">
@@ -2180,7 +2375,7 @@
         <v>81</v>
       </c>
       <c r="G21" s="29"/>
-      <c r="H21" s="20"/>
+      <c r="H21" s="37"/>
     </row>
     <row r="22" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A22" s="14" t="s">
@@ -2202,7 +2397,7 @@
         <v>103</v>
       </c>
       <c r="G22" s="29"/>
-      <c r="H22" s="20"/>
+      <c r="H22" s="37"/>
     </row>
     <row r="23" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A23" s="14" t="s">
@@ -2224,7 +2419,7 @@
         <v>103</v>
       </c>
       <c r="G23" s="29"/>
-      <c r="H23" s="20"/>
+      <c r="H23" s="37"/>
     </row>
     <row r="24" spans="1:8" s="2" customFormat="1" ht="25.5">
       <c r="A24" s="14" t="s">
@@ -2244,7 +2439,7 @@
         <v>110</v>
       </c>
       <c r="G24" s="29"/>
-      <c r="H24" s="20"/>
+      <c r="H24" s="37"/>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1">
       <c r="A25" s="14" t="s">
@@ -2305,14 +2500,14 @@
     </row>
     <row r="30" spans="1:8" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A30" s="19"/>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
       <c r="H30" s="20"/>
     </row>
     <row r="31" spans="1:8" s="2" customFormat="1" ht="12.75" customHeight="1">
@@ -2681,24 +2876,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>164</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -2707,14 +2902,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -2723,10 +2918,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -2735,22 +2930,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="49"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -2759,10 +2954,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -2771,14 +2966,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -2876,7 +3071,7 @@
       <c r="C14" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="D14" s="34" t="s">
         <v>166</v>
       </c>
       <c r="E14" t="s">
@@ -2969,24 +3164,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -2995,14 +3190,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -3011,10 +3206,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -3023,22 +3218,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="49"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -3047,10 +3242,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -3059,14 +3254,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -3283,24 +3478,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -3309,14 +3504,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -3325,10 +3520,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -3337,22 +3532,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="49"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -3361,10 +3556,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -3373,14 +3568,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -3599,24 +3794,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -3625,14 +3820,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -3641,10 +3836,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -3653,22 +3848,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="49"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -3677,10 +3872,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -3689,14 +3884,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -3898,8 +4093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3913,24 +4108,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -3939,14 +4134,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="49"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="56"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -3955,10 +4150,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -3967,22 +4162,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="49"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -3991,10 +4186,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -4003,14 +4198,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -4210,72 +4405,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G19"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4289,24 +4422,1669 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="54"/>
+      <c r="E2" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A3" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="56"/>
+      <c r="E3" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="33"/>
+    </row>
+    <row r="6" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A6" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="21">
+        <v>42626</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+    </row>
+    <row r="10" spans="1:7" ht="25.5">
+      <c r="A10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="25.5">
+      <c r="A11" s="10">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="25.5">
+      <c r="A12" s="10">
+        <v>2</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="25.5">
+      <c r="A13" s="10">
+        <v>3</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="25.5">
+      <c r="A14" s="24">
+        <v>4</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="25.5">
+      <c r="A15" s="24">
+        <v>5</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="25.5">
+      <c r="A16" s="24">
+        <v>6</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="38.25">
+      <c r="A17" s="24">
+        <v>7</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B5"/>
+    <mergeCell ref="C3:D5"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="C6:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A2" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="54"/>
+      <c r="E2" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A3" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="56"/>
+      <c r="E3" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="33"/>
+    </row>
+    <row r="6" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A6" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="21">
+        <v>42626</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+    </row>
+    <row r="10" spans="1:7" ht="25.5">
+      <c r="A10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="25.5">
+      <c r="A11" s="10">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="25.5">
+      <c r="A12" s="10">
+        <v>2</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="25.5">
+      <c r="A13" s="10">
+        <v>3</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="25.5">
+      <c r="A14" s="24">
+        <v>4</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="25.5">
+      <c r="A15" s="24">
+        <v>5</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="25.5">
+      <c r="A16" s="24">
+        <v>6</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="38.25">
+      <c r="A17" s="24">
+        <v>7</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B5"/>
+    <mergeCell ref="C3:D5"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="C6:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A2" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="54"/>
+      <c r="E2" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A3" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="56"/>
+      <c r="E3" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="33"/>
+    </row>
+    <row r="6" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A6" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="21">
+        <v>42626</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+    </row>
+    <row r="10" spans="1:7" ht="25.5">
+      <c r="A10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="25.5">
+      <c r="A11" s="10">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="25.5">
+      <c r="A12" s="10">
+        <v>2</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="76.5">
+      <c r="A13" s="10">
+        <v>3</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="25.5">
+      <c r="A14" s="24">
+        <v>4</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="25.5">
+      <c r="A15" s="24">
+        <v>5</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="25.5">
+      <c r="A16" s="24">
+        <v>6</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="25.5">
+      <c r="A17" s="24">
+        <v>7</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B5"/>
+    <mergeCell ref="C3:D5"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="C6:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A2" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="54"/>
+      <c r="E2" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A3" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="56"/>
+      <c r="E3" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="33"/>
+    </row>
+    <row r="6" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A6" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="21">
+        <v>42626</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+    </row>
+    <row r="10" spans="1:7" ht="25.5">
+      <c r="A10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="25.5">
+      <c r="A11" s="10">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="25.5">
+      <c r="A12" s="10">
+        <v>2</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="165.75">
+      <c r="A13" s="10">
+        <v>3</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="25.5">
+      <c r="A14" s="24">
+        <v>4</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="25.5">
+      <c r="A15" s="10">
+        <v>5</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="25.5">
+      <c r="A16" s="24">
+        <v>6</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16" s="27"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="25.5">
+      <c r="A17" s="10">
+        <v>7</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="25.5">
+      <c r="A18" s="24">
+        <v>8</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="25.5">
+      <c r="A19" s="10">
+        <v>9</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="24">
+        <v>10</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" spans="1:7" ht="25.5">
+      <c r="A21" s="24">
+        <v>11</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="24"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="24"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B5"/>
+    <mergeCell ref="C3:D5"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="C6:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A2" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="54"/>
+      <c r="E2" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A3" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="56"/>
+      <c r="E3" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="33"/>
+    </row>
+    <row r="6" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A6" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="21">
+        <v>42626</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+    </row>
+    <row r="10" spans="1:7" ht="25.5">
+      <c r="A10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="25.5">
+      <c r="A11" s="10">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="51">
+      <c r="A12" s="10">
+        <v>2</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="89.25">
+      <c r="A13" s="10">
+        <v>3</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="25.5">
+      <c r="A14" s="24">
+        <v>4</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="25.5">
+      <c r="A15" s="10">
+        <v>5</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="25.5">
+      <c r="A16" s="24">
+        <v>6</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="10"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B5"/>
+    <mergeCell ref="C3:D5"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="C6:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A2" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="8" t="s">
         <v>16</v>
       </c>
@@ -4315,14 +6093,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
@@ -4331,10 +6109,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="8" t="s">
         <v>22</v>
       </c>
@@ -4343,22 +6121,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="49"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="8" t="s">
         <v>18</v>
       </c>
@@ -4367,10 +6145,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="8" t="s">
         <v>23</v>
       </c>
@@ -4379,14 +6157,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -4586,24 +6364,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="8" t="s">
         <v>16</v>
       </c>
@@ -4612,14 +6390,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
@@ -4628,10 +6406,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="8" t="s">
         <v>22</v>
       </c>
@@ -4640,22 +6418,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="49"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="8" t="s">
         <v>18</v>
       </c>
@@ -4664,10 +6442,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="8" t="s">
         <v>23</v>
       </c>
@@ -4676,14 +6454,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -4874,7 +6652,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C16" sqref="C16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4888,24 +6666,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="8" t="s">
         <v>16</v>
       </c>
@@ -4914,14 +6692,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
@@ -4930,10 +6708,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="8" t="s">
         <v>22</v>
       </c>
@@ -4942,22 +6720,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="49"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="8" t="s">
         <v>18</v>
       </c>
@@ -4966,10 +6744,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="8" t="s">
         <v>23</v>
       </c>
@@ -4978,14 +6756,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -5204,24 +6982,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -5230,14 +7008,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -5246,10 +7024,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -5258,22 +7036,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="49"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -5282,10 +7060,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -5294,14 +7072,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -5514,24 +7292,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -5540,14 +7318,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -5556,10 +7334,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -5568,22 +7346,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="49"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -5592,10 +7370,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -5604,14 +7382,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -5824,24 +7602,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -5850,14 +7628,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -5866,10 +7644,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -5878,22 +7656,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="49"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -5902,10 +7680,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -5914,14 +7692,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -6100,24 +7878,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -6126,14 +7904,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -6142,10 +7920,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -6154,22 +7932,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="49"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -6178,10 +7956,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -6190,14 +7968,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -6292,10 +8070,10 @@
       <c r="B14" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="D14" s="51" t="s">
+      <c r="D14" s="35" t="s">
         <v>154</v>
       </c>
       <c r="E14" s="15" t="s">
@@ -6402,24 +8180,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -6428,14 +8206,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -6444,10 +8222,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -6456,22 +8234,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="49"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -6480,10 +8258,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -6492,14 +8270,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">

</xml_diff>

<commit_message>
LwiValidationHandler pontositas, LwiProxyHandler csak forwardol a belso reverse proxy fele
</commit_message>
<xml_diff>
--- a/other/doc/Lightweight_Integration_TEST_v1_0.xlsx
+++ b/other/doc/Lightweight_Integration_TEST_v1_0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-195" yWindow="780" windowWidth="12795" windowHeight="4785" tabRatio="853"/>
+    <workbookView xWindow="-195" yWindow="780" windowWidth="16095" windowHeight="7500" tabRatio="853"/>
   </bookViews>
   <sheets>
     <sheet name="Test_summary" sheetId="49" r:id="rId1"/>
@@ -1004,7 +1004,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="28">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1130,12 +1130,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="42"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1435,7 +1429,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1533,9 +1527,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1938,8 +1929,8 @@
   </sheetPr>
   <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="12.75"/>
@@ -1957,49 +1948,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" customFormat="1" ht="21" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="45"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:8" customFormat="1" ht="21" customHeight="1">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="50" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="51"/>
+      <c r="D2" s="50"/>
       <c r="E2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="40"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:8" customFormat="1">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="50" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="51"/>
+      <c r="D3" s="50"/>
       <c r="E3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="41">
+      <c r="F3" s="40">
         <v>42624</v>
       </c>
-      <c r="G3" s="42"/>
+      <c r="G3" s="41"/>
     </row>
     <row r="4" spans="1:8" customFormat="1" ht="12" customHeight="1">
       <c r="A4" s="5"/>
@@ -2011,15 +2002,15 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="9" t="s">
@@ -2067,7 +2058,7 @@
         <v>102</v>
       </c>
       <c r="G7" s="29"/>
-      <c r="H7" s="37"/>
+      <c r="H7" s="36"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="38.25">
       <c r="A8" s="14" t="s">
@@ -2089,7 +2080,7 @@
         <v>41</v>
       </c>
       <c r="G8" s="29"/>
-      <c r="H8" s="37"/>
+      <c r="H8" s="36"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="76.5">
       <c r="A9" s="14" t="s">
@@ -2111,7 +2102,7 @@
         <v>42</v>
       </c>
       <c r="G9" s="29"/>
-      <c r="H9" s="37"/>
+      <c r="H9" s="36"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="76.5">
       <c r="A10" s="14" t="s">
@@ -2133,7 +2124,7 @@
         <v>42</v>
       </c>
       <c r="G10" s="29"/>
-      <c r="H10" s="37"/>
+      <c r="H10" s="36"/>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="76.5">
       <c r="A11" s="14" t="s">
@@ -2155,7 +2146,7 @@
         <v>42</v>
       </c>
       <c r="G11" s="29"/>
-      <c r="H11" s="37"/>
+      <c r="H11" s="36"/>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A12" s="14" t="s">
@@ -2177,7 +2168,7 @@
         <v>58</v>
       </c>
       <c r="G12" s="29"/>
-      <c r="H12" s="37"/>
+      <c r="H12" s="36"/>
     </row>
     <row r="13" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A13" s="14" t="s">
@@ -2221,7 +2212,7 @@
         <v>70</v>
       </c>
       <c r="G14" s="29"/>
-      <c r="H14" s="37"/>
+      <c r="H14" s="36"/>
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" ht="102">
       <c r="A15" s="14" t="s">
@@ -2243,7 +2234,7 @@
         <v>70</v>
       </c>
       <c r="G15" s="29"/>
-      <c r="H15" s="37"/>
+      <c r="H15" s="36"/>
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A16" s="14" t="s">
@@ -2287,7 +2278,7 @@
         <v>81</v>
       </c>
       <c r="G17" s="29"/>
-      <c r="H17" s="37"/>
+      <c r="H17" s="36"/>
     </row>
     <row r="18" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A18" s="14" t="s">
@@ -2309,7 +2300,7 @@
         <v>81</v>
       </c>
       <c r="G18" s="29"/>
-      <c r="H18" s="37"/>
+      <c r="H18" s="36"/>
     </row>
     <row r="19" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A19" s="14" t="s">
@@ -2331,7 +2322,7 @@
         <v>81</v>
       </c>
       <c r="G19" s="29"/>
-      <c r="H19" s="37"/>
+      <c r="H19" s="36"/>
     </row>
     <row r="20" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A20" s="14" t="s">
@@ -2353,7 +2344,7 @@
         <v>81</v>
       </c>
       <c r="G20" s="11"/>
-      <c r="H20" s="37"/>
+      <c r="H20" s="36"/>
     </row>
     <row r="21" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A21" s="14" t="s">
@@ -2375,7 +2366,7 @@
         <v>81</v>
       </c>
       <c r="G21" s="29"/>
-      <c r="H21" s="37"/>
+      <c r="H21" s="36"/>
     </row>
     <row r="22" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A22" s="14" t="s">
@@ -2397,7 +2388,7 @@
         <v>103</v>
       </c>
       <c r="G22" s="29"/>
-      <c r="H22" s="37"/>
+      <c r="H22" s="36"/>
     </row>
     <row r="23" spans="1:8" s="2" customFormat="1" ht="51">
       <c r="A23" s="14" t="s">
@@ -2419,7 +2410,7 @@
         <v>103</v>
       </c>
       <c r="G23" s="29"/>
-      <c r="H23" s="37"/>
+      <c r="H23" s="36"/>
     </row>
     <row r="24" spans="1:8" s="2" customFormat="1" ht="25.5">
       <c r="A24" s="14" t="s">
@@ -2439,7 +2430,7 @@
         <v>110</v>
       </c>
       <c r="G24" s="29"/>
-      <c r="H24" s="37"/>
+      <c r="H24" s="36"/>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1">
       <c r="A25" s="14" t="s">
@@ -2500,14 +2491,14 @@
     </row>
     <row r="30" spans="1:8" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A30" s="19"/>
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
       <c r="H30" s="20"/>
     </row>
     <row r="31" spans="1:8" s="2" customFormat="1" ht="12.75" customHeight="1">
@@ -2876,24 +2867,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>164</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -2902,14 +2893,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -2918,10 +2909,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -2930,22 +2921,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -2954,10 +2945,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -2966,14 +2957,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -3164,24 +3155,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -3190,14 +3181,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -3206,10 +3197,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -3218,22 +3209,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -3242,10 +3233,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -3254,14 +3245,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -3478,24 +3469,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -3504,14 +3495,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -3520,10 +3511,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -3532,22 +3523,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -3556,10 +3547,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -3568,14 +3559,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -3794,24 +3785,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -3820,14 +3811,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -3836,10 +3827,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -3848,22 +3839,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -3872,10 +3863,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -3884,14 +3875,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -4108,24 +4099,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -4134,14 +4125,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>186</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -4150,10 +4141,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -4162,22 +4153,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -4186,10 +4177,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -4198,14 +4189,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -4422,24 +4413,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="31" t="s">
         <v>16</v>
       </c>
@@ -4448,14 +4439,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="31" t="s">
         <v>4</v>
       </c>
@@ -4464,10 +4455,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="31" t="s">
         <v>22</v>
       </c>
@@ -4476,22 +4467,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="31" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="33"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="31" t="s">
         <v>18</v>
       </c>
@@ -4500,10 +4491,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="31" t="s">
         <v>23</v>
       </c>
@@ -4512,14 +4503,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -4739,24 +4730,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="31" t="s">
         <v>16</v>
       </c>
@@ -4765,14 +4756,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="31" t="s">
         <v>4</v>
       </c>
@@ -4781,10 +4772,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="31" t="s">
         <v>22</v>
       </c>
@@ -4793,22 +4784,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="31" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="33"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="31" t="s">
         <v>18</v>
       </c>
@@ -4817,10 +4808,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="31" t="s">
         <v>23</v>
       </c>
@@ -4829,14 +4820,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -5053,24 +5044,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="31" t="s">
         <v>16</v>
       </c>
@@ -5079,14 +5070,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="31" t="s">
         <v>4</v>
       </c>
@@ -5095,10 +5086,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="31" t="s">
         <v>22</v>
       </c>
@@ -5107,22 +5098,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="31" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="33"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="31" t="s">
         <v>18</v>
       </c>
@@ -5131,10 +5122,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="31" t="s">
         <v>23</v>
       </c>
@@ -5143,14 +5134,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -5365,24 +5356,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="31" t="s">
         <v>16</v>
       </c>
@@ -5391,14 +5382,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="31" t="s">
         <v>4</v>
       </c>
@@ -5407,10 +5398,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="31" t="s">
         <v>22</v>
       </c>
@@ -5419,22 +5410,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="31" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="33"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="31" t="s">
         <v>18</v>
       </c>
@@ -5443,10 +5434,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="31" t="s">
         <v>23</v>
       </c>
@@ -5455,14 +5446,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -5767,24 +5758,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="31" t="s">
         <v>16</v>
       </c>
@@ -5793,14 +5784,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="31" t="s">
         <v>4</v>
       </c>
@@ -5809,10 +5800,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="31" t="s">
         <v>22</v>
       </c>
@@ -5821,22 +5812,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="31" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="33"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="31" t="s">
         <v>18</v>
       </c>
@@ -5845,10 +5836,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="31" t="s">
         <v>23</v>
       </c>
@@ -5857,14 +5848,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -6067,24 +6058,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="8" t="s">
         <v>16</v>
       </c>
@@ -6093,14 +6084,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
@@ -6109,10 +6100,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="8" t="s">
         <v>22</v>
       </c>
@@ -6121,22 +6112,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="8" t="s">
         <v>18</v>
       </c>
@@ -6145,10 +6136,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="8" t="s">
         <v>23</v>
       </c>
@@ -6157,14 +6148,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -6364,24 +6355,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="8" t="s">
         <v>16</v>
       </c>
@@ -6390,14 +6381,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
@@ -6406,10 +6397,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="8" t="s">
         <v>22</v>
       </c>
@@ -6418,22 +6409,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="8" t="s">
         <v>18</v>
       </c>
@@ -6442,10 +6433,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="8" t="s">
         <v>23</v>
       </c>
@@ -6454,14 +6445,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -6666,24 +6657,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="8" t="s">
         <v>16</v>
       </c>
@@ -6692,14 +6683,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
@@ -6708,10 +6699,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="8" t="s">
         <v>22</v>
       </c>
@@ -6720,22 +6711,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="8" t="s">
         <v>18</v>
       </c>
@@ -6744,10 +6735,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="8" t="s">
         <v>23</v>
       </c>
@@ -6756,14 +6747,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -6982,24 +6973,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -7008,14 +6999,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -7024,10 +7015,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -7036,22 +7027,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -7060,10 +7051,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -7072,14 +7063,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -7292,24 +7283,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -7318,14 +7309,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -7334,10 +7325,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -7346,22 +7337,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -7370,10 +7361,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -7382,14 +7373,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -7602,24 +7593,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -7628,14 +7619,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -7644,10 +7635,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -7656,22 +7647,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -7680,10 +7671,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -7692,14 +7683,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -7878,24 +7869,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -7904,14 +7895,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -7920,10 +7911,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -7932,22 +7923,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -7956,10 +7947,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -7968,14 +7959,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">
@@ -8180,24 +8171,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
@@ -8206,14 +8197,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
@@ -8222,10 +8213,10 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="28" t="s">
         <v>22</v>
       </c>
@@ -8234,22 +8225,22 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="56"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="28" t="s">
         <v>18</v>
       </c>
@@ -8258,10 +8249,10 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="55"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
@@ -8270,14 +8261,14 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="9" t="s">

</xml_diff>